<commit_message>
29.06.2018_Commit after adding the completed scenarios for Petco and Petco RD Orders .. All Payment are covered except Multiple Payments
</commit_message>
<xml_diff>
--- a/Resources/XML/XML Templates/XML.xlsx
+++ b/Resources/XML/XML Templates/XML.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="151">
   <si>
     <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t>&lt;Order AllocationRuleID="DEFAULT" BuyerUserId="rh@petco.com" CustomerEMailID= CustomerRewardsNo="511932955" Division="0" DocumentType="0001" EnterpriseCode="PETCOCOMUS" EntryType="WCS" OrderDate="" OrderType="STANDARD" PriorityCode="" SearchCriteria1="rh@petco.com" SearchCriteria2="151015" SellerOrganizationCode="PETCOCOMUS" TaxExemptFlag="" TaxPayerId="" PaymentStatus='AUTHORIZED'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Extn ExtnCIMID="" ExtnIsIlogVerified="" ExtnIsRepeatDelivery=/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1063,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="157.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1078,7 @@
     </row>
     <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>